<commit_message>
fix, add 2 districts
</commit_message>
<xml_diff>
--- a/other-formats/yemen-info.xlsx
+++ b/other-formats/yemen-info.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1472" uniqueCount="1472">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="1477">
   <x:si>
     <x:t>english_name</x:t>
   </x:si>
@@ -3370,12 +3370,18 @@
     <x:t>حَضْرَمَوْت</x:t>
   </x:si>
   <x:si>
+    <x:t>Al-Mokalla City</x:t>
+  </x:si>
+  <x:si>
+    <x:t>مدينة المكلا</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Al-Mokalla</x:t>
+  </x:si>
+  <x:si>
     <x:t>المكلا</x:t>
   </x:si>
   <x:si>
-    <x:t>Al-Mokalla</x:t>
-  </x:si>
-  <x:si>
     <x:t>المُكَلَّا</x:t>
   </x:si>
   <x:si>
@@ -3674,6 +3680,15 @@
   </x:si>
   <x:si>
     <x:t>حريضه</x:t>
+  </x:si>
+  <x:si>
+    <x:t>مَدِيْنَة المُكَلَّا</x:t>
+  </x:si>
+  <x:si>
+    <x:t>مدينه المكلا</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Al Mokalla City</x:t>
   </x:si>
   <x:si>
     <x:t>Al-Maharah</x:t>
@@ -4780,7 +4795,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:AZ332"/>
+  <x:dimension ref="A1:AZ334"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -10276,1395 +10291,1395 @@
       </x:c>
     </x:row>
     <x:row r="245" spans="1:52">
-      <x:c r="AL245" s="0" t="s">
+      <x:c r="AU245" s="0" t="s">
+        <x:v>195</x:v>
+      </x:c>
+      <x:c r="AV245" s="0" t="s">
+        <x:v>1060</x:v>
+      </x:c>
+      <x:c r="AW245" s="0" t="s">
+        <x:v>1061</x:v>
+      </x:c>
+      <x:c r="AX245" s="0" t="s">
+        <x:v>1062</x:v>
+      </x:c>
+      <x:c r="AY245" s="0" t="s">
+        <x:v>1065</x:v>
+      </x:c>
+      <x:c r="AZ245" s="0" t="s">
+        <x:v>1066</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="246" spans="1:52">
+      <x:c r="AL246" s="0" t="s">
         <x:v>200</x:v>
       </x:c>
-      <x:c r="AM245" s="0" t="s">
+      <x:c r="AM246" s="0" t="s">
         <x:v>1115</x:v>
       </x:c>
-      <x:c r="AN245" s="0" t="s">
+      <x:c r="AN246" s="0" t="s">
         <x:v>1116</x:v>
       </x:c>
-      <x:c r="AO245" s="0" t="s">
+      <x:c r="AO246" s="0" t="s">
         <x:v>1117</x:v>
       </x:c>
-      <x:c r="AP245" s="0" t="s">
+      <x:c r="AP246" s="0" t="s">
         <x:v>849</x:v>
       </x:c>
-      <x:c r="AQ245" s="0" t="s">
+      <x:c r="AQ246" s="0" t="s">
         <x:v>1118</x:v>
       </x:c>
-      <x:c r="AR245" s="0" t="s">
+      <x:c r="AR246" s="0" t="s">
         <x:v>1119</x:v>
       </x:c>
-      <x:c r="AS245" s="0" t="s">
+      <x:c r="AS246" s="0" t="s">
         <x:v>1116</x:v>
       </x:c>
-      <x:c r="AT245" s="0" t="s">
+      <x:c r="AT246" s="0" t="s">
         <x:v>1115</x:v>
       </x:c>
-      <x:c r="AU245" s="0" t="s">
+      <x:c r="AU246" s="0" t="s">
         <x:v>84</x:v>
       </x:c>
-      <x:c r="AV245" s="0" t="s">
-        <x:v>1119</x:v>
-      </x:c>
-      <x:c r="AW245" s="0" t="s">
-        <x:v>1118</x:v>
-      </x:c>
-      <x:c r="AX245" s="0" t="s">
+      <x:c r="AV246" s="0" t="s">
         <x:v>1120</x:v>
       </x:c>
-      <x:c r="AY245" s="0" t="s">
-        <x:v>1118</x:v>
-      </x:c>
-      <x:c r="AZ245" s="0" t="s">
+      <x:c r="AW246" s="0" t="s">
         <x:v>1121</x:v>
       </x:c>
-    </x:row>
-    <x:row r="246" spans="1:52">
-      <x:c r="AU246" s="0" t="s">
-        <x:v>96</x:v>
-      </x:c>
-      <x:c r="AV246" s="0" t="s">
+      <x:c r="AX246" s="0" t="s">
         <x:v>1122</x:v>
       </x:c>
-      <x:c r="AW246" s="0" t="s">
+      <x:c r="AY246" s="0" t="s">
+        <x:v>1121</x:v>
+      </x:c>
+      <x:c r="AZ246" s="0" t="s">
         <x:v>1123</x:v>
-      </x:c>
-      <x:c r="AX246" s="0" t="s">
-        <x:v>1124</x:v>
-      </x:c>
-      <x:c r="AY246" s="0" t="s">
-        <x:v>1123</x:v>
-      </x:c>
-      <x:c r="AZ246" s="0" t="s">
-        <x:v>1122</x:v>
       </x:c>
     </x:row>
     <x:row r="247" spans="1:52">
       <x:c r="AU247" s="0" t="s">
-        <x:v>100</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="AV247" s="0" t="s">
+        <x:v>1124</x:v>
+      </x:c>
+      <x:c r="AW247" s="0" t="s">
         <x:v>1125</x:v>
       </x:c>
-      <x:c r="AW247" s="0" t="s">
+      <x:c r="AX247" s="0" t="s">
         <x:v>1126</x:v>
       </x:c>
-      <x:c r="AX247" s="0" t="s">
-        <x:v>1127</x:v>
-      </x:c>
       <x:c r="AY247" s="0" t="s">
-        <x:v>1126</x:v>
+        <x:v>1125</x:v>
       </x:c>
       <x:c r="AZ247" s="0" t="s">
-        <x:v>1128</x:v>
+        <x:v>1124</x:v>
       </x:c>
     </x:row>
     <x:row r="248" spans="1:52">
       <x:c r="AU248" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="AV248" s="0" t="s">
+        <x:v>1127</x:v>
+      </x:c>
+      <x:c r="AW248" s="0" t="s">
+        <x:v>1128</x:v>
+      </x:c>
+      <x:c r="AX248" s="0" t="s">
         <x:v>1129</x:v>
       </x:c>
-      <x:c r="AW248" s="0" t="s">
+      <x:c r="AY248" s="0" t="s">
+        <x:v>1128</x:v>
+      </x:c>
+      <x:c r="AZ248" s="0" t="s">
         <x:v>1130</x:v>
-      </x:c>
-      <x:c r="AX248" s="0" t="s">
-        <x:v>1131</x:v>
-      </x:c>
-      <x:c r="AY248" s="0" t="s">
-        <x:v>1130</x:v>
-      </x:c>
-      <x:c r="AZ248" s="0" t="s">
-        <x:v>1129</x:v>
       </x:c>
     </x:row>
     <x:row r="249" spans="1:52">
       <x:c r="AU249" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="AV249" s="0" t="s">
+        <x:v>1131</x:v>
+      </x:c>
+      <x:c r="AW249" s="0" t="s">
         <x:v>1132</x:v>
       </x:c>
-      <x:c r="AW249" s="0" t="s">
+      <x:c r="AX249" s="0" t="s">
         <x:v>1133</x:v>
       </x:c>
-      <x:c r="AX249" s="0" t="s">
-        <x:v>1134</x:v>
-      </x:c>
       <x:c r="AY249" s="0" t="s">
-        <x:v>1133</x:v>
+        <x:v>1132</x:v>
       </x:c>
       <x:c r="AZ249" s="0" t="s">
-        <x:v>1132</x:v>
+        <x:v>1131</x:v>
       </x:c>
     </x:row>
     <x:row r="250" spans="1:52">
       <x:c r="AU250" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="AV250" s="0" t="s">
+        <x:v>1134</x:v>
+      </x:c>
+      <x:c r="AW250" s="0" t="s">
         <x:v>1135</x:v>
       </x:c>
-      <x:c r="AW250" s="0" t="s">
+      <x:c r="AX250" s="0" t="s">
         <x:v>1136</x:v>
       </x:c>
-      <x:c r="AX250" s="0" t="s">
-        <x:v>1137</x:v>
-      </x:c>
       <x:c r="AY250" s="0" t="s">
-        <x:v>1136</x:v>
+        <x:v>1135</x:v>
       </x:c>
       <x:c r="AZ250" s="0" t="s">
-        <x:v>1138</x:v>
+        <x:v>1134</x:v>
       </x:c>
     </x:row>
     <x:row r="251" spans="1:52">
       <x:c r="AU251" s="0" t="s">
-        <x:v>122</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="AV251" s="0" t="s">
+        <x:v>1137</x:v>
+      </x:c>
+      <x:c r="AW251" s="0" t="s">
+        <x:v>1138</x:v>
+      </x:c>
+      <x:c r="AX251" s="0" t="s">
         <x:v>1139</x:v>
       </x:c>
-      <x:c r="AW251" s="0" t="s">
+      <x:c r="AY251" s="0" t="s">
+        <x:v>1138</x:v>
+      </x:c>
+      <x:c r="AZ251" s="0" t="s">
         <x:v>1140</x:v>
-      </x:c>
-      <x:c r="AX251" s="0" t="s">
-        <x:v>1141</x:v>
-      </x:c>
-      <x:c r="AY251" s="0" t="s">
-        <x:v>1140</x:v>
-      </x:c>
-      <x:c r="AZ251" s="0" t="s">
-        <x:v>1142</x:v>
       </x:c>
     </x:row>
     <x:row r="252" spans="1:52">
       <x:c r="AU252" s="0" t="s">
-        <x:v>127</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="AV252" s="0" t="s">
+        <x:v>1141</x:v>
+      </x:c>
+      <x:c r="AW252" s="0" t="s">
+        <x:v>1142</x:v>
+      </x:c>
+      <x:c r="AX252" s="0" t="s">
         <x:v>1143</x:v>
       </x:c>
-      <x:c r="AW252" s="0" t="s">
+      <x:c r="AY252" s="0" t="s">
+        <x:v>1142</x:v>
+      </x:c>
+      <x:c r="AZ252" s="0" t="s">
         <x:v>1144</x:v>
-      </x:c>
-      <x:c r="AX252" s="0" t="s">
-        <x:v>1145</x:v>
-      </x:c>
-      <x:c r="AY252" s="0" t="s">
-        <x:v>1144</x:v>
-      </x:c>
-      <x:c r="AZ252" s="0" t="s">
-        <x:v>1143</x:v>
       </x:c>
     </x:row>
     <x:row r="253" spans="1:52">
       <x:c r="AU253" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="AV253" s="0" t="s">
+        <x:v>1145</x:v>
+      </x:c>
+      <x:c r="AW253" s="0" t="s">
         <x:v>1146</x:v>
       </x:c>
-      <x:c r="AW253" s="0" t="s">
+      <x:c r="AX253" s="0" t="s">
         <x:v>1147</x:v>
       </x:c>
-      <x:c r="AX253" s="0" t="s">
-        <x:v>1148</x:v>
-      </x:c>
       <x:c r="AY253" s="0" t="s">
-        <x:v>1147</x:v>
+        <x:v>1146</x:v>
       </x:c>
       <x:c r="AZ253" s="0" t="s">
-        <x:v>1146</x:v>
+        <x:v>1145</x:v>
       </x:c>
     </x:row>
     <x:row r="254" spans="1:52">
       <x:c r="AU254" s="0" t="s">
-        <x:v>137</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="AV254" s="0" t="s">
+        <x:v>1148</x:v>
+      </x:c>
+      <x:c r="AW254" s="0" t="s">
         <x:v>1149</x:v>
       </x:c>
-      <x:c r="AW254" s="0" t="s">
+      <x:c r="AX254" s="0" t="s">
         <x:v>1150</x:v>
       </x:c>
-      <x:c r="AX254" s="0" t="s">
-        <x:v>1151</x:v>
-      </x:c>
       <x:c r="AY254" s="0" t="s">
-        <x:v>1152</x:v>
+        <x:v>1149</x:v>
       </x:c>
       <x:c r="AZ254" s="0" t="s">
-        <x:v>1153</x:v>
+        <x:v>1148</x:v>
       </x:c>
     </x:row>
     <x:row r="255" spans="1:52">
       <x:c r="AU255" s="0" t="s">
-        <x:v>179</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="AV255" s="0" t="s">
+        <x:v>1151</x:v>
+      </x:c>
+      <x:c r="AW255" s="0" t="s">
+        <x:v>1152</x:v>
+      </x:c>
+      <x:c r="AX255" s="0" t="s">
+        <x:v>1153</x:v>
+      </x:c>
+      <x:c r="AY255" s="0" t="s">
         <x:v>1154</x:v>
       </x:c>
-      <x:c r="AW255" s="0" t="s">
+      <x:c r="AZ255" s="0" t="s">
         <x:v>1155</x:v>
-      </x:c>
-      <x:c r="AX255" s="0" t="s">
-        <x:v>1156</x:v>
-      </x:c>
-      <x:c r="AY255" s="0" t="s">
-        <x:v>1155</x:v>
-      </x:c>
-      <x:c r="AZ255" s="0" t="s">
-        <x:v>1154</x:v>
       </x:c>
     </x:row>
     <x:row r="256" spans="1:52">
       <x:c r="AU256" s="0" t="s">
-        <x:v>183</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="AV256" s="0" t="s">
+        <x:v>1156</x:v>
+      </x:c>
+      <x:c r="AW256" s="0" t="s">
         <x:v>1157</x:v>
       </x:c>
-      <x:c r="AW256" s="0" t="s">
+      <x:c r="AX256" s="0" t="s">
         <x:v>1158</x:v>
       </x:c>
-      <x:c r="AX256" s="0" t="s">
-        <x:v>1159</x:v>
-      </x:c>
       <x:c r="AY256" s="0" t="s">
-        <x:v>1158</x:v>
+        <x:v>1157</x:v>
       </x:c>
       <x:c r="AZ256" s="0" t="s">
-        <x:v>1160</x:v>
+        <x:v>1156</x:v>
       </x:c>
     </x:row>
     <x:row r="257" spans="1:52">
       <x:c r="AU257" s="0" t="s">
-        <x:v>189</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="AV257" s="0" t="s">
+        <x:v>1159</x:v>
+      </x:c>
+      <x:c r="AW257" s="0" t="s">
+        <x:v>1160</x:v>
+      </x:c>
+      <x:c r="AX257" s="0" t="s">
         <x:v>1161</x:v>
       </x:c>
-      <x:c r="AW257" s="0" t="s">
+      <x:c r="AY257" s="0" t="s">
+        <x:v>1160</x:v>
+      </x:c>
+      <x:c r="AZ257" s="0" t="s">
         <x:v>1162</x:v>
-      </x:c>
-      <x:c r="AX257" s="0" t="s">
-        <x:v>1163</x:v>
-      </x:c>
-      <x:c r="AY257" s="0" t="s">
-        <x:v>1164</x:v>
-      </x:c>
-      <x:c r="AZ257" s="0" t="s">
-        <x:v>1165</x:v>
       </x:c>
     </x:row>
     <x:row r="258" spans="1:52">
       <x:c r="AU258" s="0" t="s">
-        <x:v>195</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="AV258" s="0" t="s">
+        <x:v>1163</x:v>
+      </x:c>
+      <x:c r="AW258" s="0" t="s">
+        <x:v>1164</x:v>
+      </x:c>
+      <x:c r="AX258" s="0" t="s">
+        <x:v>1165</x:v>
+      </x:c>
+      <x:c r="AY258" s="0" t="s">
         <x:v>1166</x:v>
       </x:c>
-      <x:c r="AW258" s="0" t="s">
+      <x:c r="AZ258" s="0" t="s">
         <x:v>1167</x:v>
-      </x:c>
-      <x:c r="AX258" s="0" t="s">
-        <x:v>1168</x:v>
-      </x:c>
-      <x:c r="AY258" s="0" t="s">
-        <x:v>1167</x:v>
-      </x:c>
-      <x:c r="AZ258" s="0" t="s">
-        <x:v>1169</x:v>
       </x:c>
     </x:row>
     <x:row r="259" spans="1:52">
       <x:c r="AU259" s="0" t="s">
-        <x:v>200</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="AV259" s="0" t="s">
+        <x:v>1168</x:v>
+      </x:c>
+      <x:c r="AW259" s="0" t="s">
+        <x:v>1169</x:v>
+      </x:c>
+      <x:c r="AX259" s="0" t="s">
         <x:v>1170</x:v>
       </x:c>
-      <x:c r="AW259" s="0" t="s">
+      <x:c r="AY259" s="0" t="s">
+        <x:v>1169</x:v>
+      </x:c>
+      <x:c r="AZ259" s="0" t="s">
         <x:v>1171</x:v>
-      </x:c>
-      <x:c r="AX259" s="0" t="s">
-        <x:v>1172</x:v>
-      </x:c>
-      <x:c r="AY259" s="0" t="s">
-        <x:v>1171</x:v>
-      </x:c>
-      <x:c r="AZ259" s="0" t="s">
-        <x:v>1173</x:v>
       </x:c>
     </x:row>
     <x:row r="260" spans="1:52">
       <x:c r="AU260" s="0" t="s">
-        <x:v>204</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="AV260" s="0" t="s">
+        <x:v>1172</x:v>
+      </x:c>
+      <x:c r="AW260" s="0" t="s">
+        <x:v>1173</x:v>
+      </x:c>
+      <x:c r="AX260" s="0" t="s">
         <x:v>1174</x:v>
       </x:c>
-      <x:c r="AW260" s="0" t="s">
+      <x:c r="AY260" s="0" t="s">
+        <x:v>1173</x:v>
+      </x:c>
+      <x:c r="AZ260" s="0" t="s">
         <x:v>1175</x:v>
-      </x:c>
-      <x:c r="AX260" s="0" t="s">
-        <x:v>1176</x:v>
-      </x:c>
-      <x:c r="AY260" s="0" t="s">
-        <x:v>1175</x:v>
-      </x:c>
-      <x:c r="AZ260" s="0" t="s">
-        <x:v>1174</x:v>
       </x:c>
     </x:row>
     <x:row r="261" spans="1:52">
       <x:c r="AU261" s="0" t="s">
-        <x:v>321</x:v>
+        <x:v>204</x:v>
       </x:c>
       <x:c r="AV261" s="0" t="s">
+        <x:v>1176</x:v>
+      </x:c>
+      <x:c r="AW261" s="0" t="s">
         <x:v>1177</x:v>
       </x:c>
-      <x:c r="AW261" s="0" t="s">
+      <x:c r="AX261" s="0" t="s">
         <x:v>1178</x:v>
       </x:c>
-      <x:c r="AX261" s="0" t="s">
-        <x:v>1179</x:v>
-      </x:c>
       <x:c r="AY261" s="0" t="s">
-        <x:v>1178</x:v>
+        <x:v>1177</x:v>
       </x:c>
       <x:c r="AZ261" s="0" t="s">
-        <x:v>1177</x:v>
+        <x:v>1176</x:v>
       </x:c>
     </x:row>
     <x:row r="262" spans="1:52">
       <x:c r="AU262" s="0" t="s">
-        <x:v>327</x:v>
+        <x:v>321</x:v>
       </x:c>
       <x:c r="AV262" s="0" t="s">
+        <x:v>1179</x:v>
+      </x:c>
+      <x:c r="AW262" s="0" t="s">
         <x:v>1180</x:v>
       </x:c>
-      <x:c r="AW262" s="0" t="s">
+      <x:c r="AX262" s="0" t="s">
         <x:v>1181</x:v>
       </x:c>
-      <x:c r="AX262" s="0" t="s">
-        <x:v>1182</x:v>
-      </x:c>
       <x:c r="AY262" s="0" t="s">
-        <x:v>1181</x:v>
+        <x:v>1180</x:v>
       </x:c>
       <x:c r="AZ262" s="0" t="s">
-        <x:v>1183</x:v>
+        <x:v>1179</x:v>
       </x:c>
     </x:row>
     <x:row r="263" spans="1:52">
       <x:c r="AU263" s="0" t="s">
-        <x:v>333</x:v>
+        <x:v>327</x:v>
       </x:c>
       <x:c r="AV263" s="0" t="s">
+        <x:v>1182</x:v>
+      </x:c>
+      <x:c r="AW263" s="0" t="s">
+        <x:v>1183</x:v>
+      </x:c>
+      <x:c r="AX263" s="0" t="s">
         <x:v>1184</x:v>
       </x:c>
-      <x:c r="AW263" s="0" t="s">
+      <x:c r="AY263" s="0" t="s">
+        <x:v>1183</x:v>
+      </x:c>
+      <x:c r="AZ263" s="0" t="s">
         <x:v>1185</x:v>
-      </x:c>
-      <x:c r="AX263" s="0" t="s">
-        <x:v>1186</x:v>
-      </x:c>
-      <x:c r="AY263" s="0" t="s">
-        <x:v>1185</x:v>
-      </x:c>
-      <x:c r="AZ263" s="0" t="s">
-        <x:v>1184</x:v>
       </x:c>
     </x:row>
     <x:row r="264" spans="1:52">
       <x:c r="AU264" s="0" t="s">
-        <x:v>338</x:v>
+        <x:v>333</x:v>
       </x:c>
       <x:c r="AV264" s="0" t="s">
+        <x:v>1186</x:v>
+      </x:c>
+      <x:c r="AW264" s="0" t="s">
         <x:v>1187</x:v>
       </x:c>
-      <x:c r="AW264" s="0" t="s">
+      <x:c r="AX264" s="0" t="s">
         <x:v>1188</x:v>
       </x:c>
-      <x:c r="AX264" s="0" t="s">
-        <x:v>1189</x:v>
-      </x:c>
       <x:c r="AY264" s="0" t="s">
-        <x:v>1190</x:v>
+        <x:v>1187</x:v>
       </x:c>
       <x:c r="AZ264" s="0" t="s">
-        <x:v>1191</x:v>
+        <x:v>1186</x:v>
       </x:c>
     </x:row>
     <x:row r="265" spans="1:52">
       <x:c r="AU265" s="0" t="s">
-        <x:v>343</x:v>
+        <x:v>338</x:v>
       </x:c>
       <x:c r="AV265" s="0" t="s">
+        <x:v>1189</x:v>
+      </x:c>
+      <x:c r="AW265" s="0" t="s">
+        <x:v>1190</x:v>
+      </x:c>
+      <x:c r="AX265" s="0" t="s">
+        <x:v>1191</x:v>
+      </x:c>
+      <x:c r="AY265" s="0" t="s">
         <x:v>1192</x:v>
       </x:c>
-      <x:c r="AW265" s="0" t="s">
+      <x:c r="AZ265" s="0" t="s">
         <x:v>1193</x:v>
-      </x:c>
-      <x:c r="AX265" s="0" t="s">
-        <x:v>1194</x:v>
-      </x:c>
-      <x:c r="AY265" s="0" t="s">
-        <x:v>1195</x:v>
-      </x:c>
-      <x:c r="AZ265" s="0" t="s">
-        <x:v>1192</x:v>
       </x:c>
     </x:row>
     <x:row r="266" spans="1:52">
       <x:c r="AU266" s="0" t="s">
-        <x:v>348</x:v>
+        <x:v>343</x:v>
       </x:c>
       <x:c r="AV266" s="0" t="s">
+        <x:v>1194</x:v>
+      </x:c>
+      <x:c r="AW266" s="0" t="s">
+        <x:v>1195</x:v>
+      </x:c>
+      <x:c r="AX266" s="0" t="s">
         <x:v>1196</x:v>
-      </x:c>
-      <x:c r="AW266" s="0" t="s">
-        <x:v>1197</x:v>
-      </x:c>
-      <x:c r="AX266" s="0" t="s">
-        <x:v>1198</x:v>
       </x:c>
       <x:c r="AY266" s="0" t="s">
         <x:v>1197</x:v>
       </x:c>
       <x:c r="AZ266" s="0" t="s">
-        <x:v>1199</x:v>
+        <x:v>1194</x:v>
       </x:c>
     </x:row>
     <x:row r="267" spans="1:52">
       <x:c r="AU267" s="0" t="s">
-        <x:v>352</x:v>
+        <x:v>348</x:v>
       </x:c>
       <x:c r="AV267" s="0" t="s">
+        <x:v>1198</x:v>
+      </x:c>
+      <x:c r="AW267" s="0" t="s">
+        <x:v>1199</x:v>
+      </x:c>
+      <x:c r="AX267" s="0" t="s">
         <x:v>1200</x:v>
       </x:c>
-      <x:c r="AW267" s="0" t="s">
+      <x:c r="AY267" s="0" t="s">
+        <x:v>1199</x:v>
+      </x:c>
+      <x:c r="AZ267" s="0" t="s">
         <x:v>1201</x:v>
-      </x:c>
-      <x:c r="AX267" s="0" t="s">
-        <x:v>1202</x:v>
-      </x:c>
-      <x:c r="AY267" s="0" t="s">
-        <x:v>1201</x:v>
-      </x:c>
-      <x:c r="AZ267" s="0" t="s">
-        <x:v>1203</x:v>
       </x:c>
     </x:row>
     <x:row r="268" spans="1:52">
       <x:c r="AU268" s="0" t="s">
-        <x:v>357</x:v>
+        <x:v>352</x:v>
       </x:c>
       <x:c r="AV268" s="0" t="s">
+        <x:v>1202</x:v>
+      </x:c>
+      <x:c r="AW268" s="0" t="s">
+        <x:v>1203</x:v>
+      </x:c>
+      <x:c r="AX268" s="0" t="s">
         <x:v>1204</x:v>
       </x:c>
-      <x:c r="AW268" s="0" t="s">
+      <x:c r="AY268" s="0" t="s">
+        <x:v>1203</x:v>
+      </x:c>
+      <x:c r="AZ268" s="0" t="s">
         <x:v>1205</x:v>
-      </x:c>
-      <x:c r="AX268" s="0" t="s">
-        <x:v>1206</x:v>
-      </x:c>
-      <x:c r="AY268" s="0" t="s">
-        <x:v>1205</x:v>
-      </x:c>
-      <x:c r="AZ268" s="0" t="s">
-        <x:v>1207</x:v>
       </x:c>
     </x:row>
     <x:row r="269" spans="1:52">
       <x:c r="AU269" s="0" t="s">
-        <x:v>361</x:v>
+        <x:v>357</x:v>
       </x:c>
       <x:c r="AV269" s="0" t="s">
+        <x:v>1206</x:v>
+      </x:c>
+      <x:c r="AW269" s="0" t="s">
+        <x:v>1207</x:v>
+      </x:c>
+      <x:c r="AX269" s="0" t="s">
         <x:v>1208</x:v>
       </x:c>
-      <x:c r="AW269" s="0" t="s">
+      <x:c r="AY269" s="0" t="s">
+        <x:v>1207</x:v>
+      </x:c>
+      <x:c r="AZ269" s="0" t="s">
         <x:v>1209</x:v>
-      </x:c>
-      <x:c r="AX269" s="0" t="s">
-        <x:v>1210</x:v>
-      </x:c>
-      <x:c r="AY269" s="0" t="s">
-        <x:v>1211</x:v>
-      </x:c>
-      <x:c r="AZ269" s="0" t="s">
-        <x:v>1212</x:v>
       </x:c>
     </x:row>
     <x:row r="270" spans="1:52">
       <x:c r="AU270" s="0" t="s">
-        <x:v>366</x:v>
+        <x:v>361</x:v>
       </x:c>
       <x:c r="AV270" s="0" t="s">
+        <x:v>1210</x:v>
+      </x:c>
+      <x:c r="AW270" s="0" t="s">
+        <x:v>1211</x:v>
+      </x:c>
+      <x:c r="AX270" s="0" t="s">
+        <x:v>1212</x:v>
+      </x:c>
+      <x:c r="AY270" s="0" t="s">
         <x:v>1213</x:v>
       </x:c>
-      <x:c r="AW270" s="0" t="s">
+      <x:c r="AZ270" s="0" t="s">
         <x:v>1214</x:v>
-      </x:c>
-      <x:c r="AX270" s="0" t="s">
-        <x:v>1215</x:v>
-      </x:c>
-      <x:c r="AY270" s="0" t="s">
-        <x:v>1214</x:v>
-      </x:c>
-      <x:c r="AZ270" s="0" t="s">
-        <x:v>1213</x:v>
       </x:c>
     </x:row>
     <x:row r="271" spans="1:52">
       <x:c r="AU271" s="0" t="s">
+        <x:v>366</x:v>
+      </x:c>
+      <x:c r="AV271" s="0" t="s">
+        <x:v>1215</x:v>
+      </x:c>
+      <x:c r="AW271" s="0" t="s">
+        <x:v>1216</x:v>
+      </x:c>
+      <x:c r="AX271" s="0" t="s">
+        <x:v>1217</x:v>
+      </x:c>
+      <x:c r="AY271" s="0" t="s">
+        <x:v>1216</x:v>
+      </x:c>
+      <x:c r="AZ271" s="0" t="s">
+        <x:v>1215</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="272" spans="1:52">
+      <x:c r="AU272" s="0" t="s">
         <x:v>596</x:v>
       </x:c>
-      <x:c r="AV271" s="0" t="s">
-        <x:v>1216</x:v>
-      </x:c>
-      <x:c r="AW271" s="0" t="s">
-        <x:v>1217</x:v>
-      </x:c>
-      <x:c r="AX271" s="0" t="s">
+      <x:c r="AV272" s="0" t="s">
         <x:v>1218</x:v>
       </x:c>
-      <x:c r="AY271" s="0" t="s">
+      <x:c r="AW272" s="0" t="s">
         <x:v>1219</x:v>
       </x:c>
-      <x:c r="AZ271" s="0" t="s">
-        <x:v>1216</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="272" spans="1:52">
-      <x:c r="AL272" s="0" t="s">
-        <x:v>204</x:v>
-      </x:c>
-      <x:c r="AM272" s="0" t="s">
+      <x:c r="AX272" s="0" t="s">
         <x:v>1220</x:v>
       </x:c>
-      <x:c r="AN272" s="0" t="s">
+      <x:c r="AY272" s="0" t="s">
         <x:v>1221</x:v>
       </x:c>
-      <x:c r="AO272" s="0" t="s">
-        <x:v>1222</x:v>
-      </x:c>
-      <x:c r="AP272" s="0" t="s">
-        <x:v>849</x:v>
-      </x:c>
-      <x:c r="AQ272" s="0" t="s">
-        <x:v>1223</x:v>
-      </x:c>
-      <x:c r="AR272" s="0" t="s">
-        <x:v>1224</x:v>
-      </x:c>
-      <x:c r="AS272" s="0" t="s">
-        <x:v>1225</x:v>
-      </x:c>
-      <x:c r="AT272" s="0" t="s">
-        <x:v>1226</x:v>
-      </x:c>
-      <x:c r="AU272" s="0" t="s">
-        <x:v>84</x:v>
-      </x:c>
-      <x:c r="AV272" s="0" t="s">
-        <x:v>1227</x:v>
-      </x:c>
-      <x:c r="AW272" s="0" t="s">
-        <x:v>1228</x:v>
-      </x:c>
-      <x:c r="AX272" s="0" t="s">
-        <x:v>1229</x:v>
-      </x:c>
-      <x:c r="AY272" s="0" t="s">
-        <x:v>1228</x:v>
-      </x:c>
       <x:c r="AZ272" s="0" t="s">
-        <x:v>1227</x:v>
+        <x:v>1218</x:v>
       </x:c>
     </x:row>
     <x:row r="273" spans="1:52">
       <x:c r="AU273" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>601</x:v>
       </x:c>
       <x:c r="AV273" s="0" t="s">
+        <x:v>1118</x:v>
+      </x:c>
+      <x:c r="AW273" s="0" t="s">
+        <x:v>1119</x:v>
+      </x:c>
+      <x:c r="AX273" s="0" t="s">
+        <x:v>1222</x:v>
+      </x:c>
+      <x:c r="AY273" s="0" t="s">
+        <x:v>1223</x:v>
+      </x:c>
+      <x:c r="AZ273" s="0" t="s">
+        <x:v>1224</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="274" spans="1:52">
+      <x:c r="AL274" s="0" t="s">
+        <x:v>204</x:v>
+      </x:c>
+      <x:c r="AM274" s="0" t="s">
+        <x:v>1225</x:v>
+      </x:c>
+      <x:c r="AN274" s="0" t="s">
+        <x:v>1226</x:v>
+      </x:c>
+      <x:c r="AO274" s="0" t="s">
+        <x:v>1227</x:v>
+      </x:c>
+      <x:c r="AP274" s="0" t="s">
+        <x:v>849</x:v>
+      </x:c>
+      <x:c r="AQ274" s="0" t="s">
+        <x:v>1228</x:v>
+      </x:c>
+      <x:c r="AR274" s="0" t="s">
+        <x:v>1229</x:v>
+      </x:c>
+      <x:c r="AS274" s="0" t="s">
         <x:v>1230</x:v>
       </x:c>
-      <x:c r="AW273" s="0" t="s">
+      <x:c r="AT274" s="0" t="s">
         <x:v>1231</x:v>
       </x:c>
-      <x:c r="AX273" s="0" t="s">
+      <x:c r="AU274" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="AV274" s="0" t="s">
         <x:v>1232</x:v>
       </x:c>
-      <x:c r="AY273" s="0" t="s">
-        <x:v>1231</x:v>
-      </x:c>
-      <x:c r="AZ273" s="0" t="s">
-        <x:v>1230</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="274" spans="1:52">
-      <x:c r="AU274" s="0" t="s">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="AV274" s="0" t="s">
+      <x:c r="AW274" s="0" t="s">
         <x:v>1233</x:v>
       </x:c>
-      <x:c r="AW274" s="0" t="s">
+      <x:c r="AX274" s="0" t="s">
         <x:v>1234</x:v>
       </x:c>
-      <x:c r="AX274" s="0" t="s">
-        <x:v>1235</x:v>
-      </x:c>
       <x:c r="AY274" s="0" t="s">
-        <x:v>1234</x:v>
+        <x:v>1233</x:v>
       </x:c>
       <x:c r="AZ274" s="0" t="s">
-        <x:v>1233</x:v>
+        <x:v>1232</x:v>
       </x:c>
     </x:row>
     <x:row r="275" spans="1:52">
       <x:c r="AU275" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="AV275" s="0" t="s">
+        <x:v>1235</x:v>
+      </x:c>
+      <x:c r="AW275" s="0" t="s">
         <x:v>1236</x:v>
       </x:c>
-      <x:c r="AW275" s="0" t="s">
+      <x:c r="AX275" s="0" t="s">
         <x:v>1237</x:v>
       </x:c>
-      <x:c r="AX275" s="0" t="s">
-        <x:v>1238</x:v>
-      </x:c>
       <x:c r="AY275" s="0" t="s">
-        <x:v>1237</x:v>
+        <x:v>1236</x:v>
       </x:c>
       <x:c r="AZ275" s="0" t="s">
-        <x:v>1236</x:v>
+        <x:v>1235</x:v>
       </x:c>
     </x:row>
     <x:row r="276" spans="1:52">
       <x:c r="AU276" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="AV276" s="0" t="s">
+        <x:v>1238</x:v>
+      </x:c>
+      <x:c r="AW276" s="0" t="s">
         <x:v>1239</x:v>
       </x:c>
-      <x:c r="AW276" s="0" t="s">
+      <x:c r="AX276" s="0" t="s">
         <x:v>1240</x:v>
       </x:c>
-      <x:c r="AX276" s="0" t="s">
-        <x:v>1241</x:v>
-      </x:c>
       <x:c r="AY276" s="0" t="s">
-        <x:v>1240</x:v>
+        <x:v>1239</x:v>
       </x:c>
       <x:c r="AZ276" s="0" t="s">
-        <x:v>1239</x:v>
+        <x:v>1238</x:v>
       </x:c>
     </x:row>
     <x:row r="277" spans="1:52">
       <x:c r="AU277" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="AV277" s="0" t="s">
-        <x:v>1224</x:v>
+        <x:v>1241</x:v>
       </x:c>
       <x:c r="AW277" s="0" t="s">
-        <x:v>1223</x:v>
+        <x:v>1242</x:v>
       </x:c>
       <x:c r="AX277" s="0" t="s">
+        <x:v>1243</x:v>
+      </x:c>
+      <x:c r="AY277" s="0" t="s">
         <x:v>1242</x:v>
       </x:c>
-      <x:c r="AY277" s="0" t="s">
-        <x:v>1243</x:v>
-      </x:c>
       <x:c r="AZ277" s="0" t="s">
-        <x:v>1244</x:v>
+        <x:v>1241</x:v>
       </x:c>
     </x:row>
     <x:row r="278" spans="1:52">
       <x:c r="AU278" s="0" t="s">
-        <x:v>122</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="AV278" s="0" t="s">
+        <x:v>1244</x:v>
+      </x:c>
+      <x:c r="AW278" s="0" t="s">
         <x:v>1245</x:v>
       </x:c>
-      <x:c r="AW278" s="0" t="s">
+      <x:c r="AX278" s="0" t="s">
         <x:v>1246</x:v>
       </x:c>
-      <x:c r="AX278" s="0" t="s">
-        <x:v>1247</x:v>
-      </x:c>
       <x:c r="AY278" s="0" t="s">
-        <x:v>1246</x:v>
+        <x:v>1245</x:v>
       </x:c>
       <x:c r="AZ278" s="0" t="s">
-        <x:v>1245</x:v>
+        <x:v>1244</x:v>
       </x:c>
     </x:row>
     <x:row r="279" spans="1:52">
       <x:c r="AU279" s="0" t="s">
-        <x:v>127</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="AV279" s="0" t="s">
+        <x:v>1229</x:v>
+      </x:c>
+      <x:c r="AW279" s="0" t="s">
+        <x:v>1228</x:v>
+      </x:c>
+      <x:c r="AX279" s="0" t="s">
+        <x:v>1247</x:v>
+      </x:c>
+      <x:c r="AY279" s="0" t="s">
         <x:v>1248</x:v>
       </x:c>
-      <x:c r="AW279" s="0" t="s">
+      <x:c r="AZ279" s="0" t="s">
         <x:v>1249</x:v>
-      </x:c>
-      <x:c r="AX279" s="0" t="s">
-        <x:v>1250</x:v>
-      </x:c>
-      <x:c r="AY279" s="0" t="s">
-        <x:v>1251</x:v>
-      </x:c>
-      <x:c r="AZ279" s="0" t="s">
-        <x:v>1252</x:v>
       </x:c>
     </x:row>
     <x:row r="280" spans="1:52">
       <x:c r="AU280" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="AV280" s="0" t="s">
+        <x:v>1250</x:v>
+      </x:c>
+      <x:c r="AW280" s="0" t="s">
+        <x:v>1251</x:v>
+      </x:c>
+      <x:c r="AX280" s="0" t="s">
+        <x:v>1252</x:v>
+      </x:c>
+      <x:c r="AY280" s="0" t="s">
+        <x:v>1251</x:v>
+      </x:c>
+      <x:c r="AZ280" s="0" t="s">
+        <x:v>1250</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="281" spans="1:52">
+      <x:c r="AU281" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="AV281" s="0" t="s">
         <x:v>1253</x:v>
       </x:c>
-      <x:c r="AW280" s="0" t="s">
+      <x:c r="AW281" s="0" t="s">
         <x:v>1254</x:v>
       </x:c>
-      <x:c r="AX280" s="0" t="s">
+      <x:c r="AX281" s="0" t="s">
         <x:v>1255</x:v>
       </x:c>
-      <x:c r="AY280" s="0" t="s">
-        <x:v>1254</x:v>
-      </x:c>
-      <x:c r="AZ280" s="0" t="s">
+      <x:c r="AY281" s="0" t="s">
         <x:v>1256</x:v>
       </x:c>
-    </x:row>
-    <x:row r="281" spans="1:52">
-      <x:c r="AL281" s="0" t="s">
-        <x:v>321</x:v>
-      </x:c>
-      <x:c r="AM281" s="0" t="s">
+      <x:c r="AZ281" s="0" t="s">
         <x:v>1257</x:v>
-      </x:c>
-      <x:c r="AN281" s="0" t="s">
-        <x:v>1258</x:v>
-      </x:c>
-      <x:c r="AO281" s="0" t="s">
-        <x:v>1259</x:v>
-      </x:c>
-      <x:c r="AP281" s="0" t="s">
-        <x:v>211</x:v>
-      </x:c>
-      <x:c r="AQ281" s="0" t="s">
-        <x:v>1260</x:v>
-      </x:c>
-      <x:c r="AR281" s="0" t="s">
-        <x:v>1261</x:v>
-      </x:c>
-      <x:c r="AS281" s="0" t="s">
-        <x:v>1258</x:v>
-      </x:c>
-      <x:c r="AT281" s="0" t="s">
-        <x:v>1262</x:v>
-      </x:c>
-      <x:c r="AU281" s="0" t="s">
-        <x:v>84</x:v>
-      </x:c>
-      <x:c r="AV281" s="0" t="s">
-        <x:v>1263</x:v>
-      </x:c>
-      <x:c r="AW281" s="0" t="s">
-        <x:v>1264</x:v>
-      </x:c>
-      <x:c r="AX281" s="0" t="s">
-        <x:v>1265</x:v>
-      </x:c>
-      <x:c r="AY281" s="0" t="s">
-        <x:v>1266</x:v>
-      </x:c>
-      <x:c r="AZ281" s="0" t="s">
-        <x:v>1267</x:v>
       </x:c>
     </x:row>
     <x:row r="282" spans="1:52">
       <x:c r="AU282" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="AV282" s="0" t="s">
+        <x:v>1258</x:v>
+      </x:c>
+      <x:c r="AW282" s="0" t="s">
+        <x:v>1259</x:v>
+      </x:c>
+      <x:c r="AX282" s="0" t="s">
+        <x:v>1260</x:v>
+      </x:c>
+      <x:c r="AY282" s="0" t="s">
+        <x:v>1259</x:v>
+      </x:c>
+      <x:c r="AZ282" s="0" t="s">
+        <x:v>1261</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="283" spans="1:52">
+      <x:c r="AL283" s="0" t="s">
+        <x:v>321</x:v>
+      </x:c>
+      <x:c r="AM283" s="0" t="s">
+        <x:v>1262</x:v>
+      </x:c>
+      <x:c r="AN283" s="0" t="s">
+        <x:v>1263</x:v>
+      </x:c>
+      <x:c r="AO283" s="0" t="s">
+        <x:v>1264</x:v>
+      </x:c>
+      <x:c r="AP283" s="0" t="s">
+        <x:v>211</x:v>
+      </x:c>
+      <x:c r="AQ283" s="0" t="s">
+        <x:v>1265</x:v>
+      </x:c>
+      <x:c r="AR283" s="0" t="s">
+        <x:v>1266</x:v>
+      </x:c>
+      <x:c r="AS283" s="0" t="s">
+        <x:v>1263</x:v>
+      </x:c>
+      <x:c r="AT283" s="0" t="s">
+        <x:v>1267</x:v>
+      </x:c>
+      <x:c r="AU283" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="AV283" s="0" t="s">
         <x:v>1268</x:v>
       </x:c>
-      <x:c r="AW282" s="0" t="s">
+      <x:c r="AW283" s="0" t="s">
         <x:v>1269</x:v>
       </x:c>
-      <x:c r="AX282" s="0" t="s">
+      <x:c r="AX283" s="0" t="s">
         <x:v>1270</x:v>
       </x:c>
-      <x:c r="AY282" s="0" t="s">
-        <x:v>1269</x:v>
-      </x:c>
-      <x:c r="AZ282" s="0" t="s">
+      <x:c r="AY283" s="0" t="s">
         <x:v>1271</x:v>
       </x:c>
-    </x:row>
-    <x:row r="283" spans="1:52">
-      <x:c r="AU283" s="0" t="s">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="AV283" s="0" t="s">
+      <x:c r="AZ283" s="0" t="s">
         <x:v>1272</x:v>
-      </x:c>
-      <x:c r="AW283" s="0" t="s">
-        <x:v>1273</x:v>
-      </x:c>
-      <x:c r="AX283" s="0" t="s">
-        <x:v>1274</x:v>
-      </x:c>
-      <x:c r="AY283" s="0" t="s">
-        <x:v>1273</x:v>
-      </x:c>
-      <x:c r="AZ283" s="0" t="s">
-        <x:v>1275</x:v>
       </x:c>
     </x:row>
     <x:row r="284" spans="1:52">
       <x:c r="AU284" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="AV284" s="0" t="s">
+        <x:v>1273</x:v>
+      </x:c>
+      <x:c r="AW284" s="0" t="s">
+        <x:v>1274</x:v>
+      </x:c>
+      <x:c r="AX284" s="0" t="s">
+        <x:v>1275</x:v>
+      </x:c>
+      <x:c r="AY284" s="0" t="s">
+        <x:v>1274</x:v>
+      </x:c>
+      <x:c r="AZ284" s="0" t="s">
         <x:v>1276</x:v>
-      </x:c>
-      <x:c r="AW284" s="0" t="s">
-        <x:v>1277</x:v>
-      </x:c>
-      <x:c r="AX284" s="0" t="s">
-        <x:v>1278</x:v>
-      </x:c>
-      <x:c r="AY284" s="0" t="s">
-        <x:v>1277</x:v>
-      </x:c>
-      <x:c r="AZ284" s="0" t="s">
-        <x:v>1279</x:v>
       </x:c>
     </x:row>
     <x:row r="285" spans="1:52">
       <x:c r="AU285" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="AV285" s="0" t="s">
-        <x:v>1257</x:v>
+        <x:v>1277</x:v>
       </x:c>
       <x:c r="AW285" s="0" t="s">
-        <x:v>1258</x:v>
+        <x:v>1278</x:v>
       </x:c>
       <x:c r="AX285" s="0" t="s">
-        <x:v>1259</x:v>
+        <x:v>1279</x:v>
       </x:c>
       <x:c r="AY285" s="0" t="s">
-        <x:v>1258</x:v>
+        <x:v>1278</x:v>
       </x:c>
       <x:c r="AZ285" s="0" t="s">
-        <x:v>1262</x:v>
+        <x:v>1280</x:v>
       </x:c>
     </x:row>
     <x:row r="286" spans="1:52">
       <x:c r="AU286" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="AV286" s="0" t="s">
-        <x:v>1280</x:v>
+        <x:v>1281</x:v>
       </x:c>
       <x:c r="AW286" s="0" t="s">
-        <x:v>1281</x:v>
+        <x:v>1282</x:v>
       </x:c>
       <x:c r="AX286" s="0" t="s">
+        <x:v>1283</x:v>
+      </x:c>
+      <x:c r="AY286" s="0" t="s">
         <x:v>1282</x:v>
       </x:c>
-      <x:c r="AY286" s="0" t="s">
-        <x:v>1281</x:v>
-      </x:c>
       <x:c r="AZ286" s="0" t="s">
-        <x:v>1280</x:v>
+        <x:v>1284</x:v>
       </x:c>
     </x:row>
     <x:row r="287" spans="1:52">
       <x:c r="AU287" s="0" t="s">
-        <x:v>122</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="AV287" s="0" t="s">
-        <x:v>1283</x:v>
+        <x:v>1262</x:v>
       </x:c>
       <x:c r="AW287" s="0" t="s">
-        <x:v>1284</x:v>
+        <x:v>1263</x:v>
       </x:c>
       <x:c r="AX287" s="0" t="s">
-        <x:v>1285</x:v>
+        <x:v>1264</x:v>
       </x:c>
       <x:c r="AY287" s="0" t="s">
-        <x:v>1284</x:v>
+        <x:v>1263</x:v>
       </x:c>
       <x:c r="AZ287" s="0" t="s">
-        <x:v>1283</x:v>
+        <x:v>1267</x:v>
       </x:c>
     </x:row>
     <x:row r="288" spans="1:52">
       <x:c r="AU288" s="0" t="s">
-        <x:v>127</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="AV288" s="0" t="s">
+        <x:v>1285</x:v>
+      </x:c>
+      <x:c r="AW288" s="0" t="s">
         <x:v>1286</x:v>
       </x:c>
-      <x:c r="AW288" s="0" t="s">
+      <x:c r="AX288" s="0" t="s">
         <x:v>1287</x:v>
       </x:c>
-      <x:c r="AX288" s="0" t="s">
-        <x:v>1288</x:v>
-      </x:c>
       <x:c r="AY288" s="0" t="s">
-        <x:v>1287</x:v>
+        <x:v>1286</x:v>
       </x:c>
       <x:c r="AZ288" s="0" t="s">
-        <x:v>1286</x:v>
+        <x:v>1285</x:v>
       </x:c>
     </x:row>
     <x:row r="289" spans="1:52">
       <x:c r="AU289" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="AV289" s="0" t="s">
+        <x:v>1288</x:v>
+      </x:c>
+      <x:c r="AW289" s="0" t="s">
         <x:v>1289</x:v>
       </x:c>
-      <x:c r="AW289" s="0" t="s">
+      <x:c r="AX289" s="0" t="s">
         <x:v>1290</x:v>
       </x:c>
-      <x:c r="AX289" s="0" t="s">
+      <x:c r="AY289" s="0" t="s">
+        <x:v>1289</x:v>
+      </x:c>
+      <x:c r="AZ289" s="0" t="s">
+        <x:v>1288</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="290" spans="1:52">
+      <x:c r="AU290" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="AV290" s="0" t="s">
         <x:v>1291</x:v>
       </x:c>
-      <x:c r="AY289" s="0" t="s">
+      <x:c r="AW290" s="0" t="s">
         <x:v>1292</x:v>
       </x:c>
-      <x:c r="AZ289" s="0" t="s">
+      <x:c r="AX290" s="0" t="s">
         <x:v>1293</x:v>
       </x:c>
-    </x:row>
-    <x:row r="290" spans="1:52">
-      <x:c r="AL290" s="0" t="s">
-        <x:v>327</x:v>
-      </x:c>
-      <x:c r="AM290" s="0" t="s">
-        <x:v>1294</x:v>
-      </x:c>
-      <x:c r="AN290" s="0" t="s">
-        <x:v>1295</x:v>
-      </x:c>
-      <x:c r="AO290" s="0" t="s">
-        <x:v>1296</x:v>
-      </x:c>
-      <x:c r="AP290" s="0" t="s">
-        <x:v>422</x:v>
-      </x:c>
-      <x:c r="AQ290" s="0" t="s">
-        <x:v>1297</x:v>
-      </x:c>
-      <x:c r="AR290" s="0" t="s">
-        <x:v>1298</x:v>
-      </x:c>
-      <x:c r="AS290" s="0" t="s">
-        <x:v>1295</x:v>
-      </x:c>
-      <x:c r="AT290" s="0" t="s">
-        <x:v>1299</x:v>
-      </x:c>
-      <x:c r="AU290" s="0" t="s">
-        <x:v>84</x:v>
-      </x:c>
-      <x:c r="AV290" s="0" t="s">
-        <x:v>1300</x:v>
-      </x:c>
-      <x:c r="AW290" s="0" t="s">
-        <x:v>1301</x:v>
-      </x:c>
-      <x:c r="AX290" s="0" t="s">
-        <x:v>1302</x:v>
-      </x:c>
       <x:c r="AY290" s="0" t="s">
-        <x:v>1301</x:v>
+        <x:v>1292</x:v>
       </x:c>
       <x:c r="AZ290" s="0" t="s">
-        <x:v>1300</x:v>
+        <x:v>1291</x:v>
       </x:c>
     </x:row>
     <x:row r="291" spans="1:52">
       <x:c r="AU291" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="AV291" s="0" t="s">
+        <x:v>1294</x:v>
+      </x:c>
+      <x:c r="AW291" s="0" t="s">
+        <x:v>1295</x:v>
+      </x:c>
+      <x:c r="AX291" s="0" t="s">
+        <x:v>1296</x:v>
+      </x:c>
+      <x:c r="AY291" s="0" t="s">
+        <x:v>1297</x:v>
+      </x:c>
+      <x:c r="AZ291" s="0" t="s">
+        <x:v>1298</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="292" spans="1:52">
+      <x:c r="AL292" s="0" t="s">
+        <x:v>327</x:v>
+      </x:c>
+      <x:c r="AM292" s="0" t="s">
+        <x:v>1299</x:v>
+      </x:c>
+      <x:c r="AN292" s="0" t="s">
+        <x:v>1300</x:v>
+      </x:c>
+      <x:c r="AO292" s="0" t="s">
+        <x:v>1301</x:v>
+      </x:c>
+      <x:c r="AP292" s="0" t="s">
+        <x:v>422</x:v>
+      </x:c>
+      <x:c r="AQ292" s="0" t="s">
+        <x:v>1302</x:v>
+      </x:c>
+      <x:c r="AR292" s="0" t="s">
         <x:v>1303</x:v>
       </x:c>
-      <x:c r="AW291" s="0" t="s">
+      <x:c r="AS292" s="0" t="s">
+        <x:v>1300</x:v>
+      </x:c>
+      <x:c r="AT292" s="0" t="s">
         <x:v>1304</x:v>
       </x:c>
-      <x:c r="AX291" s="0" t="s">
+      <x:c r="AU292" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="AV292" s="0" t="s">
         <x:v>1305</x:v>
       </x:c>
-      <x:c r="AY291" s="0" t="s">
-        <x:v>1304</x:v>
-      </x:c>
-      <x:c r="AZ291" s="0" t="s">
+      <x:c r="AW292" s="0" t="s">
         <x:v>1306</x:v>
       </x:c>
-    </x:row>
-    <x:row r="292" spans="1:52">
-      <x:c r="AU292" s="0" t="s">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="AV292" s="0" t="s">
+      <x:c r="AX292" s="0" t="s">
         <x:v>1307</x:v>
       </x:c>
-      <x:c r="AW292" s="0" t="s">
-        <x:v>1308</x:v>
-      </x:c>
-      <x:c r="AX292" s="0" t="s">
-        <x:v>1309</x:v>
-      </x:c>
       <x:c r="AY292" s="0" t="s">
-        <x:v>1310</x:v>
+        <x:v>1306</x:v>
       </x:c>
       <x:c r="AZ292" s="0" t="s">
-        <x:v>1311</x:v>
+        <x:v>1305</x:v>
       </x:c>
     </x:row>
     <x:row r="293" spans="1:52">
       <x:c r="AU293" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="AV293" s="0" t="s">
-        <x:v>1312</x:v>
+        <x:v>1308</x:v>
       </x:c>
       <x:c r="AW293" s="0" t="s">
-        <x:v>1313</x:v>
+        <x:v>1309</x:v>
       </x:c>
       <x:c r="AX293" s="0" t="s">
-        <x:v>1314</x:v>
+        <x:v>1310</x:v>
       </x:c>
       <x:c r="AY293" s="0" t="s">
-        <x:v>1313</x:v>
+        <x:v>1309</x:v>
       </x:c>
       <x:c r="AZ293" s="0" t="s">
-        <x:v>1315</x:v>
+        <x:v>1311</x:v>
       </x:c>
     </x:row>
     <x:row r="294" spans="1:52">
       <x:c r="AU294" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="AV294" s="0" t="s">
+        <x:v>1312</x:v>
+      </x:c>
+      <x:c r="AW294" s="0" t="s">
+        <x:v>1313</x:v>
+      </x:c>
+      <x:c r="AX294" s="0" t="s">
+        <x:v>1314</x:v>
+      </x:c>
+      <x:c r="AY294" s="0" t="s">
+        <x:v>1315</x:v>
+      </x:c>
+      <x:c r="AZ294" s="0" t="s">
         <x:v>1316</x:v>
-      </x:c>
-      <x:c r="AW294" s="0" t="s">
-        <x:v>1317</x:v>
-      </x:c>
-      <x:c r="AX294" s="0" t="s">
-        <x:v>1318</x:v>
-      </x:c>
-      <x:c r="AY294" s="0" t="s">
-        <x:v>1317</x:v>
-      </x:c>
-      <x:c r="AZ294" s="0" t="s">
-        <x:v>1319</x:v>
       </x:c>
     </x:row>
     <x:row r="295" spans="1:52">
       <x:c r="AU295" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="AV295" s="0" t="s">
-        <x:v>1294</x:v>
+        <x:v>1317</x:v>
       </x:c>
       <x:c r="AW295" s="0" t="s">
-        <x:v>1295</x:v>
+        <x:v>1318</x:v>
       </x:c>
       <x:c r="AX295" s="0" t="s">
-        <x:v>1296</x:v>
+        <x:v>1319</x:v>
       </x:c>
       <x:c r="AY295" s="0" t="s">
-        <x:v>1295</x:v>
+        <x:v>1318</x:v>
       </x:c>
       <x:c r="AZ295" s="0" t="s">
-        <x:v>1299</x:v>
+        <x:v>1320</x:v>
       </x:c>
     </x:row>
     <x:row r="296" spans="1:52">
       <x:c r="AU296" s="0" t="s">
-        <x:v>122</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="AV296" s="0" t="s">
-        <x:v>1298</x:v>
+        <x:v>1321</x:v>
       </x:c>
       <x:c r="AW296" s="0" t="s">
-        <x:v>1297</x:v>
+        <x:v>1322</x:v>
       </x:c>
       <x:c r="AX296" s="0" t="s">
-        <x:v>1320</x:v>
+        <x:v>1323</x:v>
       </x:c>
       <x:c r="AY296" s="0" t="s">
-        <x:v>1321</x:v>
+        <x:v>1322</x:v>
       </x:c>
       <x:c r="AZ296" s="0" t="s">
-        <x:v>1322</x:v>
+        <x:v>1324</x:v>
       </x:c>
     </x:row>
     <x:row r="297" spans="1:52">
       <x:c r="AU297" s="0" t="s">
-        <x:v>127</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="AV297" s="0" t="s">
-        <x:v>1323</x:v>
+        <x:v>1299</x:v>
       </x:c>
       <x:c r="AW297" s="0" t="s">
-        <x:v>1324</x:v>
+        <x:v>1300</x:v>
       </x:c>
       <x:c r="AX297" s="0" t="s">
-        <x:v>1325</x:v>
+        <x:v>1301</x:v>
       </x:c>
       <x:c r="AY297" s="0" t="s">
-        <x:v>1324</x:v>
+        <x:v>1300</x:v>
       </x:c>
       <x:c r="AZ297" s="0" t="s">
-        <x:v>1323</x:v>
+        <x:v>1304</x:v>
       </x:c>
     </x:row>
     <x:row r="298" spans="1:52">
       <x:c r="AU298" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="AV298" s="0" t="s">
+        <x:v>1303</x:v>
+      </x:c>
+      <x:c r="AW298" s="0" t="s">
+        <x:v>1302</x:v>
+      </x:c>
+      <x:c r="AX298" s="0" t="s">
+        <x:v>1325</x:v>
+      </x:c>
+      <x:c r="AY298" s="0" t="s">
         <x:v>1326</x:v>
       </x:c>
-      <x:c r="AW298" s="0" t="s">
+      <x:c r="AZ298" s="0" t="s">
         <x:v>1327</x:v>
       </x:c>
-      <x:c r="AX298" s="0" t="s">
+    </x:row>
+    <x:row r="299" spans="1:52">
+      <x:c r="AU299" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="AV299" s="0" t="s">
         <x:v>1328</x:v>
       </x:c>
-      <x:c r="AY298" s="0" t="s">
-        <x:v>1327</x:v>
-      </x:c>
-      <x:c r="AZ298" s="0" t="s">
-        <x:v>1326</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="299" spans="1:52">
-      <x:c r="AL299" s="0" t="s">
-        <x:v>333</x:v>
-      </x:c>
-      <x:c r="AM299" s="0" t="s">
+      <x:c r="AW299" s="0" t="s">
         <x:v>1329</x:v>
       </x:c>
-      <x:c r="AN299" s="0" t="s">
+      <x:c r="AX299" s="0" t="s">
         <x:v>1330</x:v>
       </x:c>
-      <x:c r="AO299" s="0" t="s">
-        <x:v>1331</x:v>
-      </x:c>
-      <x:c r="AP299" s="0" t="s">
-        <x:v>211</x:v>
-      </x:c>
-      <x:c r="AQ299" s="0" t="s">
-        <x:v>1332</x:v>
-      </x:c>
-      <x:c r="AR299" s="0" t="s">
-        <x:v>1333</x:v>
-      </x:c>
-      <x:c r="AS299" s="0" t="s">
-        <x:v>1330</x:v>
-      </x:c>
-      <x:c r="AT299" s="0" t="s">
+      <x:c r="AY299" s="0" t="s">
         <x:v>1329</x:v>
       </x:c>
-      <x:c r="AU299" s="0" t="s">
-        <x:v>84</x:v>
-      </x:c>
-      <x:c r="AV299" s="0" t="s">
-        <x:v>1334</x:v>
-      </x:c>
-      <x:c r="AW299" s="0" t="s">
-        <x:v>1335</x:v>
-      </x:c>
-      <x:c r="AX299" s="0" t="s">
-        <x:v>1336</x:v>
-      </x:c>
-      <x:c r="AY299" s="0" t="s">
-        <x:v>1335</x:v>
-      </x:c>
       <x:c r="AZ299" s="0" t="s">
-        <x:v>1337</x:v>
+        <x:v>1328</x:v>
       </x:c>
     </x:row>
     <x:row r="300" spans="1:52">
       <x:c r="AU300" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="AV300" s="0" t="s">
-        <x:v>1333</x:v>
+        <x:v>1331</x:v>
       </x:c>
       <x:c r="AW300" s="0" t="s">
         <x:v>1332</x:v>
       </x:c>
       <x:c r="AX300" s="0" t="s">
+        <x:v>1333</x:v>
+      </x:c>
+      <x:c r="AY300" s="0" t="s">
+        <x:v>1332</x:v>
+      </x:c>
+      <x:c r="AZ300" s="0" t="s">
+        <x:v>1331</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="301" spans="1:52">
+      <x:c r="AL301" s="0" t="s">
+        <x:v>333</x:v>
+      </x:c>
+      <x:c r="AM301" s="0" t="s">
+        <x:v>1334</x:v>
+      </x:c>
+      <x:c r="AN301" s="0" t="s">
+        <x:v>1335</x:v>
+      </x:c>
+      <x:c r="AO301" s="0" t="s">
+        <x:v>1336</x:v>
+      </x:c>
+      <x:c r="AP301" s="0" t="s">
+        <x:v>211</x:v>
+      </x:c>
+      <x:c r="AQ301" s="0" t="s">
+        <x:v>1337</x:v>
+      </x:c>
+      <x:c r="AR301" s="0" t="s">
         <x:v>1338</x:v>
       </x:c>
-      <x:c r="AY300" s="0" t="s">
+      <x:c r="AS301" s="0" t="s">
+        <x:v>1335</x:v>
+      </x:c>
+      <x:c r="AT301" s="0" t="s">
+        <x:v>1334</x:v>
+      </x:c>
+      <x:c r="AU301" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="AV301" s="0" t="s">
         <x:v>1339</x:v>
       </x:c>
-      <x:c r="AZ300" s="0" t="s">
+      <x:c r="AW301" s="0" t="s">
         <x:v>1340</x:v>
       </x:c>
-    </x:row>
-    <x:row r="301" spans="1:52">
-      <x:c r="AU301" s="0" t="s">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="AV301" s="0" t="s">
+      <x:c r="AX301" s="0" t="s">
         <x:v>1341</x:v>
       </x:c>
-      <x:c r="AW301" s="0" t="s">
+      <x:c r="AY301" s="0" t="s">
+        <x:v>1340</x:v>
+      </x:c>
+      <x:c r="AZ301" s="0" t="s">
         <x:v>1342</x:v>
-      </x:c>
-      <x:c r="AX301" s="0" t="s">
-        <x:v>1343</x:v>
-      </x:c>
-      <x:c r="AY301" s="0" t="s">
-        <x:v>1344</x:v>
-      </x:c>
-      <x:c r="AZ301" s="0" t="s">
-        <x:v>1345</x:v>
       </x:c>
     </x:row>
     <x:row r="302" spans="1:52">
       <x:c r="AU302" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="AV302" s="0" t="s">
-        <x:v>1346</x:v>
+        <x:v>1338</x:v>
       </x:c>
       <x:c r="AW302" s="0" t="s">
-        <x:v>1347</x:v>
+        <x:v>1337</x:v>
       </x:c>
       <x:c r="AX302" s="0" t="s">
-        <x:v>1348</x:v>
+        <x:v>1343</x:v>
       </x:c>
       <x:c r="AY302" s="0" t="s">
-        <x:v>1347</x:v>
+        <x:v>1344</x:v>
       </x:c>
       <x:c r="AZ302" s="0" t="s">
-        <x:v>1349</x:v>
+        <x:v>1345</x:v>
       </x:c>
     </x:row>
     <x:row r="303" spans="1:52">
       <x:c r="AU303" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="AV303" s="0" t="s">
+        <x:v>1346</x:v>
+      </x:c>
+      <x:c r="AW303" s="0" t="s">
+        <x:v>1347</x:v>
+      </x:c>
+      <x:c r="AX303" s="0" t="s">
+        <x:v>1348</x:v>
+      </x:c>
+      <x:c r="AY303" s="0" t="s">
+        <x:v>1349</x:v>
+      </x:c>
+      <x:c r="AZ303" s="0" t="s">
         <x:v>1350</x:v>
-      </x:c>
-      <x:c r="AW303" s="0" t="s">
-        <x:v>1351</x:v>
-      </x:c>
-      <x:c r="AX303" s="0" t="s">
-        <x:v>1352</x:v>
-      </x:c>
-      <x:c r="AY303" s="0" t="s">
-        <x:v>1353</x:v>
-      </x:c>
-      <x:c r="AZ303" s="0" t="s">
-        <x:v>1354</x:v>
       </x:c>
     </x:row>
     <x:row r="304" spans="1:52">
       <x:c r="AU304" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="AV304" s="0" t="s">
-        <x:v>1355</x:v>
+        <x:v>1351</x:v>
       </x:c>
       <x:c r="AW304" s="0" t="s">
-        <x:v>1356</x:v>
+        <x:v>1352</x:v>
       </x:c>
       <x:c r="AX304" s="0" t="s">
-        <x:v>1357</x:v>
+        <x:v>1353</x:v>
       </x:c>
       <x:c r="AY304" s="0" t="s">
-        <x:v>1356</x:v>
+        <x:v>1352</x:v>
       </x:c>
       <x:c r="AZ304" s="0" t="s">
-        <x:v>1358</x:v>
+        <x:v>1354</x:v>
       </x:c>
     </x:row>
     <x:row r="305" spans="1:52">
       <x:c r="AU305" s="0" t="s">
-        <x:v>122</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="AV305" s="0" t="s">
+        <x:v>1355</x:v>
+      </x:c>
+      <x:c r="AW305" s="0" t="s">
+        <x:v>1356</x:v>
+      </x:c>
+      <x:c r="AX305" s="0" t="s">
+        <x:v>1357</x:v>
+      </x:c>
+      <x:c r="AY305" s="0" t="s">
+        <x:v>1358</x:v>
+      </x:c>
+      <x:c r="AZ305" s="0" t="s">
         <x:v>1359</x:v>
-      </x:c>
-      <x:c r="AW305" s="0" t="s">
-        <x:v>1360</x:v>
-      </x:c>
-      <x:c r="AX305" s="0" t="s">
-        <x:v>1361</x:v>
-      </x:c>
-      <x:c r="AY305" s="0" t="s">
-        <x:v>1362</x:v>
-      </x:c>
-      <x:c r="AZ305" s="0" t="s">
-        <x:v>1363</x:v>
       </x:c>
     </x:row>
     <x:row r="306" spans="1:52">
       <x:c r="AU306" s="0" t="s">
-        <x:v>127</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="AV306" s="0" t="s">
-        <x:v>1364</x:v>
+        <x:v>1360</x:v>
       </x:c>
       <x:c r="AW306" s="0" t="s">
-        <x:v>1365</x:v>
+        <x:v>1361</x:v>
       </x:c>
       <x:c r="AX306" s="0" t="s">
-        <x:v>1366</x:v>
+        <x:v>1362</x:v>
       </x:c>
       <x:c r="AY306" s="0" t="s">
-        <x:v>1365</x:v>
+        <x:v>1361</x:v>
       </x:c>
       <x:c r="AZ306" s="0" t="s">
-        <x:v>1367</x:v>
+        <x:v>1363</x:v>
       </x:c>
     </x:row>
     <x:row r="307" spans="1:52">
       <x:c r="AU307" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="AV307" s="0" t="s">
-        <x:v>1368</x:v>
+        <x:v>1364</x:v>
       </x:c>
       <x:c r="AW307" s="0" t="s">
-        <x:v>1369</x:v>
+        <x:v>1365</x:v>
       </x:c>
       <x:c r="AX307" s="0" t="s">
-        <x:v>1370</x:v>
+        <x:v>1366</x:v>
       </x:c>
       <x:c r="AY307" s="0" t="s">
-        <x:v>1369</x:v>
+        <x:v>1367</x:v>
       </x:c>
       <x:c r="AZ307" s="0" t="s">
         <x:v>1368</x:v>
@@ -11672,383 +11687,356 @@
     </x:row>
     <x:row r="308" spans="1:52">
       <x:c r="AU308" s="0" t="s">
-        <x:v>137</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="AV308" s="0" t="s">
+        <x:v>1369</x:v>
+      </x:c>
+      <x:c r="AW308" s="0" t="s">
+        <x:v>1370</x:v>
+      </x:c>
+      <x:c r="AX308" s="0" t="s">
         <x:v>1371</x:v>
       </x:c>
-      <x:c r="AW308" s="0" t="s">
+      <x:c r="AY308" s="0" t="s">
+        <x:v>1370</x:v>
+      </x:c>
+      <x:c r="AZ308" s="0" t="s">
         <x:v>1372</x:v>
-      </x:c>
-      <x:c r="AX308" s="0" t="s">
-        <x:v>1373</x:v>
-      </x:c>
-      <x:c r="AY308" s="0" t="s">
-        <x:v>1372</x:v>
-      </x:c>
-      <x:c r="AZ308" s="0" t="s">
-        <x:v>1371</x:v>
       </x:c>
     </x:row>
     <x:row r="309" spans="1:52">
       <x:c r="AU309" s="0" t="s">
-        <x:v>179</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="AV309" s="0" t="s">
+        <x:v>1373</x:v>
+      </x:c>
+      <x:c r="AW309" s="0" t="s">
         <x:v>1374</x:v>
       </x:c>
-      <x:c r="AW309" s="0" t="s">
+      <x:c r="AX309" s="0" t="s">
         <x:v>1375</x:v>
       </x:c>
-      <x:c r="AX309" s="0" t="s">
-        <x:v>1376</x:v>
-      </x:c>
       <x:c r="AY309" s="0" t="s">
-        <x:v>1375</x:v>
+        <x:v>1374</x:v>
       </x:c>
       <x:c r="AZ309" s="0" t="s">
-        <x:v>1374</x:v>
+        <x:v>1373</x:v>
       </x:c>
     </x:row>
     <x:row r="310" spans="1:52">
       <x:c r="AU310" s="0" t="s">
-        <x:v>183</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="AV310" s="0" t="s">
+        <x:v>1376</x:v>
+      </x:c>
+      <x:c r="AW310" s="0" t="s">
         <x:v>1377</x:v>
       </x:c>
-      <x:c r="AW310" s="0" t="s">
+      <x:c r="AX310" s="0" t="s">
         <x:v>1378</x:v>
       </x:c>
-      <x:c r="AX310" s="0" t="s">
-        <x:v>1379</x:v>
-      </x:c>
       <x:c r="AY310" s="0" t="s">
-        <x:v>1378</x:v>
+        <x:v>1377</x:v>
       </x:c>
       <x:c r="AZ310" s="0" t="s">
-        <x:v>1377</x:v>
+        <x:v>1376</x:v>
       </x:c>
     </x:row>
     <x:row r="311" spans="1:52">
       <x:c r="AU311" s="0" t="s">
-        <x:v>189</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="AV311" s="0" t="s">
+        <x:v>1379</x:v>
+      </x:c>
+      <x:c r="AW311" s="0" t="s">
         <x:v>1380</x:v>
       </x:c>
-      <x:c r="AW311" s="0" t="s">
+      <x:c r="AX311" s="0" t="s">
         <x:v>1381</x:v>
       </x:c>
-      <x:c r="AX311" s="0" t="s">
-        <x:v>1382</x:v>
-      </x:c>
       <x:c r="AY311" s="0" t="s">
-        <x:v>1383</x:v>
+        <x:v>1380</x:v>
       </x:c>
       <x:c r="AZ311" s="0" t="s">
-        <x:v>1384</x:v>
+        <x:v>1379</x:v>
       </x:c>
     </x:row>
     <x:row r="312" spans="1:52">
       <x:c r="AU312" s="0" t="s">
-        <x:v>195</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="AV312" s="0" t="s">
-        <x:v>1385</x:v>
+        <x:v>1382</x:v>
       </x:c>
       <x:c r="AW312" s="0" t="s">
-        <x:v>1386</x:v>
+        <x:v>1383</x:v>
       </x:c>
       <x:c r="AX312" s="0" t="s">
-        <x:v>1387</x:v>
+        <x:v>1384</x:v>
       </x:c>
       <x:c r="AY312" s="0" t="s">
-        <x:v>1386</x:v>
+        <x:v>1383</x:v>
       </x:c>
       <x:c r="AZ312" s="0" t="s">
-        <x:v>1388</x:v>
+        <x:v>1382</x:v>
       </x:c>
     </x:row>
     <x:row r="313" spans="1:52">
       <x:c r="AU313" s="0" t="s">
-        <x:v>200</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="AV313" s="0" t="s">
-        <x:v>1389</x:v>
+        <x:v>1385</x:v>
       </x:c>
       <x:c r="AW313" s="0" t="s">
-        <x:v>1390</x:v>
+        <x:v>1386</x:v>
       </x:c>
       <x:c r="AX313" s="0" t="s">
-        <x:v>1391</x:v>
+        <x:v>1387</x:v>
       </x:c>
       <x:c r="AY313" s="0" t="s">
-        <x:v>1390</x:v>
+        <x:v>1388</x:v>
       </x:c>
       <x:c r="AZ313" s="0" t="s">
         <x:v>1389</x:v>
       </x:c>
     </x:row>
     <x:row r="314" spans="1:52">
-      <x:c r="AL314" s="0" t="s">
-        <x:v>338</x:v>
-      </x:c>
-      <x:c r="AM314" s="0" t="s">
+      <x:c r="AU314" s="0" t="s">
+        <x:v>195</x:v>
+      </x:c>
+      <x:c r="AV314" s="0" t="s">
+        <x:v>1390</x:v>
+      </x:c>
+      <x:c r="AW314" s="0" t="s">
+        <x:v>1391</x:v>
+      </x:c>
+      <x:c r="AX314" s="0" t="s">
         <x:v>1392</x:v>
       </x:c>
-      <x:c r="AN314" s="0" t="s">
+      <x:c r="AY314" s="0" t="s">
+        <x:v>1391</x:v>
+      </x:c>
+      <x:c r="AZ314" s="0" t="s">
         <x:v>1393</x:v>
-      </x:c>
-      <x:c r="AO314" s="0" t="s">
-        <x:v>1394</x:v>
-      </x:c>
-      <x:c r="AP314" s="0" t="s">
-        <x:v>247</x:v>
-      </x:c>
-      <x:c r="AQ314" s="0" t="s">
-        <x:v>1395</x:v>
-      </x:c>
-      <x:c r="AR314" s="0" t="s">
-        <x:v>1396</x:v>
-      </x:c>
-      <x:c r="AS314" s="0" t="s">
-        <x:v>1397</x:v>
-      </x:c>
-      <x:c r="AT314" s="0" t="s">
-        <x:v>1392</x:v>
-      </x:c>
-      <x:c r="AU314" s="0" t="s">
-        <x:v>84</x:v>
-      </x:c>
-      <x:c r="AV314" s="0" t="s">
-        <x:v>1398</x:v>
-      </x:c>
-      <x:c r="AW314" s="0" t="s">
-        <x:v>1399</x:v>
-      </x:c>
-      <x:c r="AX314" s="0" t="s">
-        <x:v>1400</x:v>
-      </x:c>
-      <x:c r="AY314" s="0" t="s">
-        <x:v>1399</x:v>
-      </x:c>
-      <x:c r="AZ314" s="0" t="s">
-        <x:v>1401</x:v>
       </x:c>
     </x:row>
     <x:row r="315" spans="1:52">
       <x:c r="AU315" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="AV315" s="0" t="s">
+        <x:v>1394</x:v>
+      </x:c>
+      <x:c r="AW315" s="0" t="s">
+        <x:v>1395</x:v>
+      </x:c>
+      <x:c r="AX315" s="0" t="s">
+        <x:v>1396</x:v>
+      </x:c>
+      <x:c r="AY315" s="0" t="s">
+        <x:v>1395</x:v>
+      </x:c>
+      <x:c r="AZ315" s="0" t="s">
+        <x:v>1394</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="316" spans="1:52">
+      <x:c r="AL316" s="0" t="s">
+        <x:v>338</x:v>
+      </x:c>
+      <x:c r="AM316" s="0" t="s">
+        <x:v>1397</x:v>
+      </x:c>
+      <x:c r="AN316" s="0" t="s">
+        <x:v>1398</x:v>
+      </x:c>
+      <x:c r="AO316" s="0" t="s">
+        <x:v>1399</x:v>
+      </x:c>
+      <x:c r="AP316" s="0" t="s">
+        <x:v>247</x:v>
+      </x:c>
+      <x:c r="AQ316" s="0" t="s">
+        <x:v>1400</x:v>
+      </x:c>
+      <x:c r="AR316" s="0" t="s">
+        <x:v>1401</x:v>
+      </x:c>
+      <x:c r="AS316" s="0" t="s">
         <x:v>1402</x:v>
       </x:c>
-      <x:c r="AW315" s="0" t="s">
+      <x:c r="AT316" s="0" t="s">
+        <x:v>1397</x:v>
+      </x:c>
+      <x:c r="AU316" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="AV316" s="0" t="s">
         <x:v>1403</x:v>
       </x:c>
-      <x:c r="AX315" s="0" t="s">
+      <x:c r="AW316" s="0" t="s">
         <x:v>1404</x:v>
       </x:c>
-      <x:c r="AY315" s="0" t="s">
+      <x:c r="AX316" s="0" t="s">
         <x:v>1405</x:v>
       </x:c>
-      <x:c r="AZ315" s="0" t="s">
+      <x:c r="AY316" s="0" t="s">
+        <x:v>1404</x:v>
+      </x:c>
+      <x:c r="AZ316" s="0" t="s">
         <x:v>1406</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="316" spans="1:52">
-      <x:c r="AU316" s="0" t="s">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="AV316" s="0" t="s">
-        <x:v>1396</x:v>
-      </x:c>
-      <x:c r="AW316" s="0" t="s">
-        <x:v>1395</x:v>
-      </x:c>
-      <x:c r="AX316" s="0" t="s">
-        <x:v>1407</x:v>
-      </x:c>
-      <x:c r="AY316" s="0" t="s">
-        <x:v>1395</x:v>
-      </x:c>
-      <x:c r="AZ316" s="0" t="s">
-        <x:v>1408</x:v>
       </x:c>
     </x:row>
     <x:row r="317" spans="1:52">
       <x:c r="AU317" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="AV317" s="0" t="s">
+        <x:v>1407</x:v>
+      </x:c>
+      <x:c r="AW317" s="0" t="s">
+        <x:v>1408</x:v>
+      </x:c>
+      <x:c r="AX317" s="0" t="s">
         <x:v>1409</x:v>
-      </x:c>
-      <x:c r="AW317" s="0" t="s">
-        <x:v>1410</x:v>
-      </x:c>
-      <x:c r="AX317" s="0" t="s">
-        <x:v>1411</x:v>
       </x:c>
       <x:c r="AY317" s="0" t="s">
         <x:v>1410</x:v>
       </x:c>
       <x:c r="AZ317" s="0" t="s">
-        <x:v>1409</x:v>
+        <x:v>1411</x:v>
       </x:c>
     </x:row>
     <x:row r="318" spans="1:52">
       <x:c r="AU318" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="AV318" s="0" t="s">
+        <x:v>1401</x:v>
+      </x:c>
+      <x:c r="AW318" s="0" t="s">
+        <x:v>1400</x:v>
+      </x:c>
+      <x:c r="AX318" s="0" t="s">
         <x:v>1412</x:v>
       </x:c>
-      <x:c r="AW318" s="0" t="s">
+      <x:c r="AY318" s="0" t="s">
+        <x:v>1400</x:v>
+      </x:c>
+      <x:c r="AZ318" s="0" t="s">
         <x:v>1413</x:v>
-      </x:c>
-      <x:c r="AX318" s="0" t="s">
-        <x:v>1414</x:v>
-      </x:c>
-      <x:c r="AY318" s="0" t="s">
-        <x:v>1415</x:v>
-      </x:c>
-      <x:c r="AZ318" s="0" t="s">
-        <x:v>1412</x:v>
       </x:c>
     </x:row>
     <x:row r="319" spans="1:52">
       <x:c r="AU319" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="AV319" s="0" t="s">
+        <x:v>1414</x:v>
+      </x:c>
+      <x:c r="AW319" s="0" t="s">
+        <x:v>1415</x:v>
+      </x:c>
+      <x:c r="AX319" s="0" t="s">
         <x:v>1416</x:v>
       </x:c>
-      <x:c r="AW319" s="0" t="s">
+      <x:c r="AY319" s="0" t="s">
+        <x:v>1415</x:v>
+      </x:c>
+      <x:c r="AZ319" s="0" t="s">
+        <x:v>1414</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="320" spans="1:52">
+      <x:c r="AU320" s="0" t="s">
+        <x:v>111</x:v>
+      </x:c>
+      <x:c r="AV320" s="0" t="s">
         <x:v>1417</x:v>
       </x:c>
-      <x:c r="AX319" s="0" t="s">
+      <x:c r="AW320" s="0" t="s">
         <x:v>1418</x:v>
       </x:c>
-      <x:c r="AY319" s="0" t="s">
+      <x:c r="AX320" s="0" t="s">
         <x:v>1419</x:v>
       </x:c>
-      <x:c r="AZ319" s="0" t="s">
+      <x:c r="AY320" s="0" t="s">
         <x:v>1420</x:v>
       </x:c>
-    </x:row>
-    <x:row r="320" spans="1:52">
-      <x:c r="AL320" s="0" t="s">
-        <x:v>343</x:v>
-      </x:c>
-      <x:c r="AM320" s="0" t="s">
-        <x:v>1421</x:v>
-      </x:c>
-      <x:c r="AN320" s="0" t="s">
-        <x:v>1422</x:v>
-      </x:c>
-      <x:c r="AO320" s="0" t="s">
-        <x:v>1423</x:v>
-      </x:c>
-      <x:c r="AP320" s="0" t="s">
-        <x:v>849</x:v>
-      </x:c>
-      <x:c r="AQ320" s="0" t="s">
-        <x:v>1424</x:v>
-      </x:c>
-      <x:c r="AR320" s="0" t="s">
-        <x:v>1425</x:v>
-      </x:c>
-      <x:c r="AS320" s="0" t="s">
-        <x:v>1426</x:v>
-      </x:c>
-      <x:c r="AT320" s="0" t="s">
-        <x:v>1421</x:v>
-      </x:c>
-      <x:c r="AU320" s="0" t="s">
-        <x:v>84</x:v>
-      </x:c>
-      <x:c r="AV320" s="0" t="s">
-        <x:v>1425</x:v>
-      </x:c>
-      <x:c r="AW320" s="0" t="s">
-        <x:v>1424</x:v>
-      </x:c>
-      <x:c r="AX320" s="0" t="s">
-        <x:v>1427</x:v>
-      </x:c>
-      <x:c r="AY320" s="0" t="s">
-        <x:v>1424</x:v>
-      </x:c>
       <x:c r="AZ320" s="0" t="s">
-        <x:v>1425</x:v>
+        <x:v>1417</x:v>
       </x:c>
     </x:row>
     <x:row r="321" spans="1:52">
       <x:c r="AU321" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="AV321" s="0" t="s">
-        <x:v>1428</x:v>
+        <x:v>1421</x:v>
       </x:c>
       <x:c r="AW321" s="0" t="s">
-        <x:v>1429</x:v>
+        <x:v>1422</x:v>
       </x:c>
       <x:c r="AX321" s="0" t="s">
-        <x:v>1430</x:v>
+        <x:v>1423</x:v>
       </x:c>
       <x:c r="AY321" s="0" t="s">
-        <x:v>1431</x:v>
+        <x:v>1424</x:v>
       </x:c>
       <x:c r="AZ321" s="0" t="s">
-        <x:v>1432</x:v>
+        <x:v>1425</x:v>
       </x:c>
     </x:row>
     <x:row r="322" spans="1:52">
       <x:c r="AL322" s="0" t="s">
-        <x:v>348</x:v>
+        <x:v>343</x:v>
       </x:c>
       <x:c r="AM322" s="0" t="s">
-        <x:v>1433</x:v>
+        <x:v>1426</x:v>
       </x:c>
       <x:c r="AN322" s="0" t="s">
-        <x:v>1434</x:v>
+        <x:v>1427</x:v>
       </x:c>
       <x:c r="AO322" s="0" t="s">
-        <x:v>1435</x:v>
+        <x:v>1428</x:v>
       </x:c>
       <x:c r="AP322" s="0" t="s">
-        <x:v>211</x:v>
+        <x:v>849</x:v>
       </x:c>
       <x:c r="AQ322" s="0" t="s">
-        <x:v>1436</x:v>
+        <x:v>1429</x:v>
       </x:c>
       <x:c r="AR322" s="0" t="s">
-        <x:v>1437</x:v>
+        <x:v>1430</x:v>
       </x:c>
       <x:c r="AS322" s="0" t="s">
-        <x:v>1438</x:v>
+        <x:v>1431</x:v>
       </x:c>
       <x:c r="AT322" s="0" t="s">
-        <x:v>1433</x:v>
+        <x:v>1426</x:v>
       </x:c>
       <x:c r="AU322" s="0" t="s">
         <x:v>84</x:v>
       </x:c>
       <x:c r="AV322" s="0" t="s">
-        <x:v>1439</x:v>
+        <x:v>1430</x:v>
       </x:c>
       <x:c r="AW322" s="0" t="s">
-        <x:v>1440</x:v>
+        <x:v>1429</x:v>
       </x:c>
       <x:c r="AX322" s="0" t="s">
-        <x:v>1441</x:v>
+        <x:v>1432</x:v>
       </x:c>
       <x:c r="AY322" s="0" t="s">
-        <x:v>1442</x:v>
+        <x:v>1429</x:v>
       </x:c>
       <x:c r="AZ322" s="0" t="s">
-        <x:v>1439</x:v>
+        <x:v>1430</x:v>
       </x:c>
     </x:row>
     <x:row r="323" spans="1:52">
@@ -12056,67 +12044,94 @@
         <x:v>96</x:v>
       </x:c>
       <x:c r="AV323" s="0" t="s">
+        <x:v>1433</x:v>
+      </x:c>
+      <x:c r="AW323" s="0" t="s">
+        <x:v>1434</x:v>
+      </x:c>
+      <x:c r="AX323" s="0" t="s">
+        <x:v>1435</x:v>
+      </x:c>
+      <x:c r="AY323" s="0" t="s">
+        <x:v>1436</x:v>
+      </x:c>
+      <x:c r="AZ323" s="0" t="s">
+        <x:v>1437</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="324" spans="1:52">
+      <x:c r="AL324" s="0" t="s">
+        <x:v>348</x:v>
+      </x:c>
+      <x:c r="AM324" s="0" t="s">
+        <x:v>1438</x:v>
+      </x:c>
+      <x:c r="AN324" s="0" t="s">
+        <x:v>1439</x:v>
+      </x:c>
+      <x:c r="AO324" s="0" t="s">
+        <x:v>1440</x:v>
+      </x:c>
+      <x:c r="AP324" s="0" t="s">
+        <x:v>211</x:v>
+      </x:c>
+      <x:c r="AQ324" s="0" t="s">
+        <x:v>1441</x:v>
+      </x:c>
+      <x:c r="AR324" s="0" t="s">
+        <x:v>1442</x:v>
+      </x:c>
+      <x:c r="AS324" s="0" t="s">
         <x:v>1443</x:v>
       </x:c>
-      <x:c r="AW323" s="0" t="s">
+      <x:c r="AT324" s="0" t="s">
+        <x:v>1438</x:v>
+      </x:c>
+      <x:c r="AU324" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="AV324" s="0" t="s">
         <x:v>1444</x:v>
       </x:c>
-      <x:c r="AX323" s="0" t="s">
+      <x:c r="AW324" s="0" t="s">
         <x:v>1445</x:v>
       </x:c>
-      <x:c r="AY323" s="0" t="s">
-        <x:v>1444</x:v>
-      </x:c>
-      <x:c r="AZ323" s="0" t="s">
-        <x:v>1443</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="324" spans="1:52">
-      <x:c r="AU324" s="0" t="s">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="AV324" s="0" t="s">
+      <x:c r="AX324" s="0" t="s">
         <x:v>1446</x:v>
-      </x:c>
-      <x:c r="AW324" s="0" t="s">
-        <x:v>1447</x:v>
-      </x:c>
-      <x:c r="AX324" s="0" t="s">
-        <x:v>1448</x:v>
       </x:c>
       <x:c r="AY324" s="0" t="s">
         <x:v>1447</x:v>
       </x:c>
       <x:c r="AZ324" s="0" t="s">
-        <x:v>1446</x:v>
+        <x:v>1444</x:v>
       </x:c>
     </x:row>
     <x:row r="325" spans="1:52">
       <x:c r="AU325" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="AV325" s="0" t="s">
+        <x:v>1448</x:v>
+      </x:c>
+      <x:c r="AW325" s="0" t="s">
         <x:v>1449</x:v>
       </x:c>
-      <x:c r="AW325" s="0" t="s">
+      <x:c r="AX325" s="0" t="s">
         <x:v>1450</x:v>
       </x:c>
-      <x:c r="AX325" s="0" t="s">
-        <x:v>1451</x:v>
-      </x:c>
       <x:c r="AY325" s="0" t="s">
-        <x:v>1450</x:v>
+        <x:v>1449</x:v>
       </x:c>
       <x:c r="AZ325" s="0" t="s">
-        <x:v>1449</x:v>
+        <x:v>1448</x:v>
       </x:c>
     </x:row>
     <x:row r="326" spans="1:52">
       <x:c r="AU326" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="AV326" s="0" t="s">
-        <x:v>793</x:v>
+        <x:v>1451</x:v>
       </x:c>
       <x:c r="AW326" s="0" t="s">
         <x:v>1452</x:v>
@@ -12128,12 +12143,12 @@
         <x:v>1452</x:v>
       </x:c>
       <x:c r="AZ326" s="0" t="s">
-        <x:v>793</x:v>
+        <x:v>1451</x:v>
       </x:c>
     </x:row>
     <x:row r="327" spans="1:52">
       <x:c r="AU327" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="AV327" s="0" t="s">
         <x:v>1454</x:v>
@@ -12153,87 +12168,87 @@
     </x:row>
     <x:row r="328" spans="1:52">
       <x:c r="AU328" s="0" t="s">
-        <x:v>122</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="AV328" s="0" t="s">
+        <x:v>793</x:v>
+      </x:c>
+      <x:c r="AW328" s="0" t="s">
         <x:v>1457</x:v>
       </x:c>
-      <x:c r="AW328" s="0" t="s">
+      <x:c r="AX328" s="0" t="s">
         <x:v>1458</x:v>
       </x:c>
-      <x:c r="AX328" s="0" t="s">
-        <x:v>1459</x:v>
-      </x:c>
       <x:c r="AY328" s="0" t="s">
-        <x:v>1458</x:v>
+        <x:v>1457</x:v>
       </x:c>
       <x:c r="AZ328" s="0" t="s">
-        <x:v>1457</x:v>
+        <x:v>793</x:v>
       </x:c>
     </x:row>
     <x:row r="329" spans="1:52">
       <x:c r="AU329" s="0" t="s">
-        <x:v>127</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="AV329" s="0" t="s">
+        <x:v>1459</x:v>
+      </x:c>
+      <x:c r="AW329" s="0" t="s">
         <x:v>1460</x:v>
       </x:c>
-      <x:c r="AW329" s="0" t="s">
+      <x:c r="AX329" s="0" t="s">
         <x:v>1461</x:v>
       </x:c>
-      <x:c r="AX329" s="0" t="s">
-        <x:v>1462</x:v>
-      </x:c>
       <x:c r="AY329" s="0" t="s">
-        <x:v>1461</x:v>
+        <x:v>1460</x:v>
       </x:c>
       <x:c r="AZ329" s="0" t="s">
-        <x:v>1463</x:v>
+        <x:v>1459</x:v>
       </x:c>
     </x:row>
     <x:row r="330" spans="1:52">
       <x:c r="AU330" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="AV330" s="0" t="s">
+        <x:v>1462</x:v>
+      </x:c>
+      <x:c r="AW330" s="0" t="s">
+        <x:v>1463</x:v>
+      </x:c>
+      <x:c r="AX330" s="0" t="s">
         <x:v>1464</x:v>
       </x:c>
-      <x:c r="AW330" s="0" t="s">
-        <x:v>1465</x:v>
-      </x:c>
-      <x:c r="AX330" s="0" t="s">
-        <x:v>1466</x:v>
-      </x:c>
       <x:c r="AY330" s="0" t="s">
-        <x:v>1467</x:v>
+        <x:v>1463</x:v>
       </x:c>
       <x:c r="AZ330" s="0" t="s">
-        <x:v>1464</x:v>
+        <x:v>1462</x:v>
       </x:c>
     </x:row>
     <x:row r="331" spans="1:52">
       <x:c r="AU331" s="0" t="s">
-        <x:v>137</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="AV331" s="0" t="s">
-        <x:v>1437</x:v>
+        <x:v>1465</x:v>
       </x:c>
       <x:c r="AW331" s="0" t="s">
-        <x:v>1436</x:v>
+        <x:v>1466</x:v>
       </x:c>
       <x:c r="AX331" s="0" t="s">
+        <x:v>1467</x:v>
+      </x:c>
+      <x:c r="AY331" s="0" t="s">
+        <x:v>1466</x:v>
+      </x:c>
+      <x:c r="AZ331" s="0" t="s">
         <x:v>1468</x:v>
-      </x:c>
-      <x:c r="AY331" s="0" t="s">
-        <x:v>1436</x:v>
-      </x:c>
-      <x:c r="AZ331" s="0" t="s">
-        <x:v>1437</x:v>
       </x:c>
     </x:row>
     <x:row r="332" spans="1:52">
       <x:c r="AU332" s="0" t="s">
-        <x:v>179</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="AV332" s="0" t="s">
         <x:v>1469</x:v>
@@ -12245,10 +12260,50 @@
         <x:v>1471</x:v>
       </x:c>
       <x:c r="AY332" s="0" t="s">
-        <x:v>1470</x:v>
+        <x:v>1472</x:v>
       </x:c>
       <x:c r="AZ332" s="0" t="s">
         <x:v>1469</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="333" spans="1:52">
+      <x:c r="AU333" s="0" t="s">
+        <x:v>137</x:v>
+      </x:c>
+      <x:c r="AV333" s="0" t="s">
+        <x:v>1442</x:v>
+      </x:c>
+      <x:c r="AW333" s="0" t="s">
+        <x:v>1441</x:v>
+      </x:c>
+      <x:c r="AX333" s="0" t="s">
+        <x:v>1473</x:v>
+      </x:c>
+      <x:c r="AY333" s="0" t="s">
+        <x:v>1441</x:v>
+      </x:c>
+      <x:c r="AZ333" s="0" t="s">
+        <x:v>1442</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="334" spans="1:52">
+      <x:c r="AU334" s="0" t="s">
+        <x:v>179</x:v>
+      </x:c>
+      <x:c r="AV334" s="0" t="s">
+        <x:v>1474</x:v>
+      </x:c>
+      <x:c r="AW334" s="0" t="s">
+        <x:v>1475</x:v>
+      </x:c>
+      <x:c r="AX334" s="0" t="s">
+        <x:v>1476</x:v>
+      </x:c>
+      <x:c r="AY334" s="0" t="s">
+        <x:v>1475</x:v>
+      </x:c>
+      <x:c r="AZ334" s="0" t="s">
+        <x:v>1474</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>